<commit_message>
Arreglos cronograma y varios son HTTP
</commit_message>
<xml_diff>
--- a/diagramas/cronograma.xlsx
+++ b/diagramas/cronograma.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -53,9 +53,6 @@
     <t>Especificación conexiones</t>
   </si>
   <si>
-    <t>Codificacion servidores HTTPs</t>
-  </si>
-  <si>
     <t>Codificación bajo nivel</t>
   </si>
   <si>
@@ -63,13 +60,23 @@
   </si>
   <si>
     <t>SW</t>
+  </si>
+  <si>
+    <t>Codificacion comunicación TLS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -262,55 +269,53 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF00B050"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF00B050"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF00B050"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF00B050"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -319,58 +324,58 @@
   </cellStyleXfs>
   <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -690,249 +695,250 @@
   <dimension ref="A1:AB7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:J6"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="10" width="11.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="4" customWidth="1"/>
+    <col min="6" max="10" width="11.85546875" style="4" customWidth="1"/>
+    <col min="11" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="2">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1">
         <v>1</v>
       </c>
-      <c r="C1" s="2">
+      <c r="C1" s="1">
         <v>2</v>
       </c>
-      <c r="D1" s="2">
+      <c r="D1" s="1">
         <v>3</v>
       </c>
-      <c r="E1" s="3">
+      <c r="E1" s="2">
         <v>4</v>
       </c>
-      <c r="F1" s="2">
+      <c r="F1" s="1">
         <v>5</v>
       </c>
-      <c r="G1" s="2">
+      <c r="G1" s="1">
         <v>6</v>
       </c>
-      <c r="H1" s="2">
+      <c r="H1" s="1">
         <v>7</v>
       </c>
-      <c r="I1" s="2">
+      <c r="I1" s="1">
         <v>8</v>
       </c>
-      <c r="J1" s="2">
+      <c r="J1" s="1">
         <v>9</v>
       </c>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
     </row>
     <row r="2" spans="1:28" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="2" t="s">
+      <c r="G2" s="17"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
     </row>
     <row r="3" spans="1:28" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="12" t="s">
+      <c r="A3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
-      <c r="AA3" s="1"/>
-      <c r="AB3" s="1"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
     </row>
     <row r="4" spans="1:28" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="17" t="s">
+      <c r="A4" s="13"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="18"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
-      <c r="AA4" s="1"/>
-      <c r="AB4" s="1"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
     </row>
     <row r="5" spans="1:28" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="20"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="23"/>
       <c r="J5" s="11"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
-      <c r="W5" s="1"/>
-      <c r="X5" s="1"/>
-      <c r="Y5" s="1"/>
-      <c r="Z5" s="1"/>
-      <c r="AA5" s="1"/>
-      <c r="AB5" s="1"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
     </row>
     <row r="6" spans="1:28" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="4"/>
+      <c r="A6" s="14"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="5"/>
       <c r="J6" s="9"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
-      <c r="W6" s="1"/>
-      <c r="X6" s="1"/>
-      <c r="Y6" s="1"/>
-      <c r="Z6" s="1"/>
-      <c r="AA6" s="1"/>
-      <c r="AB6" s="1"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>